<commit_message>
updated data & added forecast
</commit_message>
<xml_diff>
--- a/data_output/models/model_groups.xlsx
+++ b/data_output/models/model_groups.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -372,7 +372,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Молоко питьевое цельное стерилизованное 2,5-3,2% жирности, л.RData</t>
+          <t>Масло сливочное, кг.RData</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -384,7 +384,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Масло сливочное, кг.RData</t>
+          <t>Молоко питьевое цельное пастеризованное 2,5-3,2% жирности, л.RData</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -396,7 +396,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Молоко питьевое цельное пастеризованное 2,5-3,2% жирности, л.RData</t>
+          <t>Молоко питьевое цельное стерилизованное 2,5-3,2% жирности, л.RData</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -504,12 +504,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Сахар-песок, кг.RData</t>
+          <t>Изделия из меха, шт..RData</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Прочее, продовольственное</t>
+          <t>Прочее, непродовольственное</t>
         </is>
       </c>
     </row>
@@ -534,6 +534,30 @@
       <c r="B15" t="inlineStr">
         <is>
           <t>Прочее, непродовольственное</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Фототехника, шт..RData</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Прочее, непродовольственное</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Сахар-песок, кг.RData</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Прочее, продовольственное</t>
         </is>
       </c>
     </row>

</xml_diff>